<commit_message>
saving completed 19 before slight optimization test
</commit_message>
<xml_diff>
--- a/0 NeetCode/19. Remove Nth Node From End of List/Whiteboards/Solution.xlsx
+++ b/0 NeetCode/19. Remove Nth Node From End of List/Whiteboards/Solution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 NeetCode\19. Remove Nth Node From End of List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC62FA-2BDE-4A8A-A947-F8537BAC1E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="4005" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+  <si>
+    <t>frwd</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67,7 +81,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,17 +398,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="G8:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="8" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="1">
+        <v>3</v>
+      </c>
+      <c r="V8" s="1">
+        <v>2</v>
+      </c>
+      <c r="W8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>2</v>
+      </c>
+      <c r="T9" s="1">
+        <v>3</v>
+      </c>
+      <c r="U9" s="1">
+        <v>4</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1">
+        <v>3</v>
+      </c>
+      <c r="U10" s="1">
+        <v>4</v>
+      </c>
+      <c r="V10" s="1">
+        <v>7</v>
+      </c>
+      <c r="W10" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>11</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>14</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>5</v>
+      </c>
+      <c r="T11" s="1">
+        <v>8</v>
+      </c>
+      <c r="U11" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>15</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>7</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="1">
+        <v>6</v>
+      </c>
+      <c r="S12" s="1">
+        <v>9</v>
+      </c>
+      <c r="T12" s="1">
+        <v>12</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>13</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>16</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="7:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="26:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>